<commit_message>
perubahan laporan Dil Oke2
</commit_message>
<xml_diff>
--- a/public/Pelanggan/Darmaraja_Oke.xlsx
+++ b/public/Pelanggan/Darmaraja_Oke.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riank\Downloads\OKE Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32818B70-DCC4-4D72-B873-1C0D529078AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1A9E78-ED78-4E4F-A1A9-FBBF6697CEA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{9BB69F2C-843C-4B7B-AB19-DEE24A0F072E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15429" uniqueCount="2275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15537" uniqueCount="2276">
   <si>
     <t xml:space="preserve">0304001004 </t>
   </si>
@@ -6859,6 +6859,9 @@
   </si>
   <si>
     <t>ada</t>
+  </si>
+  <si>
+    <t>2023-10-15</t>
   </si>
 </sst>
 </file>
@@ -7229,10 +7232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DAC2521-8EC4-47C3-B50F-93378100408E}">
-  <dimension ref="A1:AD1084"/>
+  <dimension ref="A1:AD1093"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1028" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q1037" sqref="Q1037"/>
+    <sheetView tabSelected="1" topLeftCell="Q1080" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y1081" sqref="Y1081"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -88236,6 +88239,537 @@
         <v>81</v>
       </c>
     </row>
+    <row r="1085" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1085">
+        <v>301007147</v>
+      </c>
+      <c r="B1085" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1085" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1085" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1085" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1085" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1085" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1085" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1085" s="5" t="s">
+        <v>2275</v>
+      </c>
+      <c r="R1085" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S1085" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="T1085" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="U1085" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1085" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W1085" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1085" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z1085" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC1085" s="1">
+        <v>33</v>
+      </c>
+      <c r="AD1085" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1086">
+        <v>303003046</v>
+      </c>
+      <c r="B1086" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1086" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1086" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1086" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1086" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1086" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1086" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1086" s="5" t="s">
+        <v>2275</v>
+      </c>
+      <c r="R1086" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S1086" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="T1086" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="U1086" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1086" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W1086" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1086" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z1086" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC1086" s="1">
+        <v>33</v>
+      </c>
+      <c r="AD1086" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1087">
+        <v>301003337</v>
+      </c>
+      <c r="B1087" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1087" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1087" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1087" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1087" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1087" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1087" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1087" s="5" t="s">
+        <v>2275</v>
+      </c>
+      <c r="R1087" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S1087" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="T1087" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="U1087" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1087" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W1087" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1087" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z1087" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC1087" s="1">
+        <v>33</v>
+      </c>
+      <c r="AD1087" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1088">
+        <v>301003338</v>
+      </c>
+      <c r="B1088" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1088" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1088" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1088" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1088" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1088" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1088" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1088" s="5" t="s">
+        <v>2275</v>
+      </c>
+      <c r="R1088" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S1088" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="T1088" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="U1088" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1088" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W1088" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1088" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z1088" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC1088" s="1">
+        <v>33</v>
+      </c>
+      <c r="AD1088" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1089">
+        <v>301005009</v>
+      </c>
+      <c r="B1089" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1089" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1089" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1089" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1089" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1089" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1089" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1089" s="5" t="s">
+        <v>2275</v>
+      </c>
+      <c r="R1089" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S1089" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="T1089" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="U1089" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1089" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W1089" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1089" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z1089" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC1089" s="1">
+        <v>33</v>
+      </c>
+      <c r="AD1089" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1090">
+        <v>301003339</v>
+      </c>
+      <c r="B1090" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1090" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1090" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1090" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1090" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1090" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1090" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1090" s="5" t="s">
+        <v>2275</v>
+      </c>
+      <c r="R1090" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S1090" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="T1090" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="U1090" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1090" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W1090" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1090" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z1090" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC1090" s="1">
+        <v>33</v>
+      </c>
+      <c r="AD1090" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1091">
+        <v>304001534</v>
+      </c>
+      <c r="B1091" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1091" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1091" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1091" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1091" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1091" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1091" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1091" s="5" t="s">
+        <v>2275</v>
+      </c>
+      <c r="R1091" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S1091" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="T1091" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="U1091" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1091" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W1091" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1091" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z1091" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC1091" s="1">
+        <v>33</v>
+      </c>
+      <c r="AD1091" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1092">
+        <v>301001071</v>
+      </c>
+      <c r="B1092" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1092" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1092" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1092" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1092" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1092" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1092" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1092" s="5" t="s">
+        <v>2275</v>
+      </c>
+      <c r="R1092" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S1092" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="T1092" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="U1092" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1092" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W1092" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1092" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z1092" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC1092" s="1">
+        <v>33</v>
+      </c>
+      <c r="AD1092" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1093">
+        <v>304001533</v>
+      </c>
+      <c r="B1093" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1093" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1093" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1093" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1093" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1093" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1093" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1093" s="5" t="s">
+        <v>2275</v>
+      </c>
+      <c r="R1093" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S1093" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="T1093" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="U1093" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1093" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W1093" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1093" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z1093" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC1093" s="1">
+        <v>33</v>
+      </c>
+      <c r="AD1093" s="1">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>